<commit_message>
Merge Look-up tables - new BC Transformer and workspace
</commit_message>
<xml_diff>
--- a/FME_files/LOOKUP_TABLES/BC_DefaultAttributeMapper.xlsx
+++ b/FME_files/LOOKUP_TABLES/BC_DefaultAttributeMapper.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
   <si>
     <t>p-t_entity</t>
   </si>
@@ -102,9 +102,6 @@
   </si>
   <si>
     <t>reference_system_version</t>
-  </si>
-  <si>
-    <t>EPSG</t>
   </si>
   <si>
     <t>unknown</t>
@@ -452,7 +449,7 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,12 +583,12 @@
         <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B17" t="s">
         <v>18</v>
@@ -599,15 +596,15 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B19" t="s">
         <v>18</v>
@@ -615,15 +612,15 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s">
         <v>18</v>
@@ -631,7 +628,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B22" t="s">
         <v>18</v>
@@ -639,7 +636,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B23" t="s">
         <v>18</v>

</xml_diff>